<commit_message>
fixed file selection issue
</commit_message>
<xml_diff>
--- a/YOLOv8-DeepSORT-Object-Tracking/ultralytics/yolo/v8/detect/output.xlsx
+++ b/YOLOv8-DeepSORT-Object-Tracking/ultralytics/yolo/v8/detect/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,11 +462,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>truck</t>
+          <t>car/taxi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,13 +477,13 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>17:59:54</t>
+          <t>02:28:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -498,7 +498,95 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>18:00:07</t>
+          <t>02:28:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>car/taxi</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>west</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>02:29:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>car/taxi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>south</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>02:29:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>car/taxi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>west</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>02:29:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>car/taxi</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>east</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>north</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>02:29:45</t>
         </is>
       </c>
     </row>

</xml_diff>